<commit_message>
Fixed predict function in X2-salinity model. Fixed salinity-zoop model Rmd to account for Eurytemora name change in zooper. Re-run all alts based on the predict function fix.
</commit_message>
<xml_diff>
--- a/Salinity_Zooplankton_analysis/Biomass conversions.xlsx
+++ b/Salinity_Zooplankton_analysis/Biomass conversions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\ZoopSynth\Data paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmahardja\Documents\GitHub\DeltaSmelt_SummerFallX2_VOI\Salinity_Zooplankton_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E8C096-A92A-4650-89A0-C853302FCD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65B7489-E829-4910-9825-159E1413AAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Micro and Meso-zooplankton" sheetId="2" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>Culver, D.A., M.M. Boucherle, D.J. Bean &amp; J.W. Fletcher. 1985. Biomass of freshwater crustacean zooplankton from length-weight regression. Can. J. Fish. aquat. Sci., 42: 1380-1390.</t>
   </si>
   <si>
-    <t>Eurytemora affinis</t>
-  </si>
-  <si>
     <t>Ambler JW, Cloern JE, Hutchinson A. 1985. Seasonal cycles of zooplankton from San Francisco Bay. Hydrobiologia. 129(1):177–197.</t>
   </si>
   <si>
@@ -312,6 +309,9 @@
   </si>
   <si>
     <t>CDFW, unpublished</t>
+  </si>
+  <si>
+    <t>Eurytemora carolleeae</t>
   </si>
 </sst>
 </file>
@@ -765,8 +765,8 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,12 +793,12 @@
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>5</v>
@@ -810,7 +810,7 @@
         <v>3.36</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -827,7 +827,7 @@
         <v>2.984</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
         <v>1.3009999999999999</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +861,7 @@
         <v>2.6659999999999999</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -878,12 +878,12 @@
         <v>1.1619999999999999</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -895,7 +895,7 @@
         <v>0.3</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -917,10 +917,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>8</v>
@@ -929,15 +929,15 @@
         <v>3</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>6</v>
@@ -946,7 +946,7 @@
         <v>1.5</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -968,10 +968,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>8</v>
@@ -980,15 +980,15 @@
         <v>1</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>8</v>
@@ -997,15 +997,15 @@
         <v>3.36</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>6</v>
@@ -1014,7 +1014,7 @@
         <v>1.68</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1082,12 +1082,12 @@
         <v>2</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>10</v>
@@ -1099,12 +1099,12 @@
         <v>3.55</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>10</v>
@@ -1116,12 +1116,12 @@
         <v>1.4430000000000001</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>10</v>
@@ -1133,18 +1133,18 @@
         <v>0.1</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>5</v>
@@ -1167,7 +1167,7 @@
         <v>0.04</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1184,7 +1184,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
         <v>0.04</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,12 +1218,12 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>10</v>
@@ -1235,12 +1235,12 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>10</v>
@@ -1252,12 +1252,12 @@
         <v>8.8663036902600939E-2</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>10</v>
@@ -1269,12 +1269,12 @@
         <v>0.04</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>5</v>
@@ -1286,12 +1286,12 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>5</v>
@@ -1303,12 +1303,12 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>10</v>
@@ -1320,12 +1320,12 @@
         <v>0.21</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>10</v>
@@ -1337,12 +1337,12 @@
         <v>0.5</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>5</v>
@@ -1354,12 +1354,12 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>5</v>
@@ -1371,12 +1371,12 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>5</v>
@@ -1388,12 +1388,12 @@
         <v>0.1</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>10</v>
@@ -1405,12 +1405,12 @@
         <v>2.6619999999999999</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>10</v>
@@ -1422,12 +1422,12 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>5</v>
@@ -1439,12 +1439,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>10</v>
@@ -1456,12 +1456,12 @@
         <v>3.4129999999999998</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>10</v>
@@ -1473,12 +1473,12 @@
         <v>1.8109999999999999</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
@@ -1490,12 +1490,12 @@
         <v>0.12</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>5</v>
@@ -1507,12 +1507,12 @@
         <v>15.89</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -1524,12 +1524,12 @@
         <v>7.95</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -1541,7 +1541,7 @@
         <v>0.12</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1585,42 +1585,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="7">
         <v>200</v>
@@ -1638,21 +1638,21 @@
         <v>2.2593000000000001</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="7">
         <v>700</v>
@@ -1670,21 +1670,21 @@
         <v>3.2532999999999999</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="7">
         <v>63</v>
@@ -1703,21 +1703,21 @@
         <v>2.57</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3">
         <v>108</v>
@@ -1735,21 +1735,21 @@
         <v>2.6458651999999998</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="3">
         <v>113</v>
@@ -1767,21 +1767,21 @@
         <v>2.8256119000000002</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="3">
         <v>25</v>
@@ -1799,21 +1799,21 @@
         <v>2.4761397999999999</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="3">
         <v>57</v>
@@ -1831,21 +1831,21 @@
         <v>2.202537</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="3">
         <v>196</v>
@@ -1863,21 +1863,21 @@
         <v>2.7388843999999999</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="3">
         <v>367</v>
@@ -1895,21 +1895,21 @@
         <v>2.8963214000000002</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="3">
         <v>599</v>
@@ -1927,21 +1927,21 @@
         <v>2.7443140000000001</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="3">
         <v>156</v>
@@ -1959,21 +1959,21 @@
         <v>2.6305483999999999</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="3">
         <v>292</v>
@@ -1991,21 +1991,21 @@
         <v>2.8436471000000001</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="3">
         <v>37</v>
@@ -2023,21 +2023,21 @@
         <v>3.2843296999999998</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="3">
         <v>209</v>
@@ -2055,21 +2055,21 @@
         <v>3.0492894000000001</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="3">
         <v>307</v>
@@ -2087,21 +2087,21 @@
         <v>2.6718519000000001</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" s="3">
         <v>84</v>
@@ -2119,21 +2119,21 @@
         <v>3.2246939999999999</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="3">
         <v>106</v>
@@ -2151,21 +2151,21 @@
         <v>3.2745017999999999</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" s="3">
         <v>39</v>
@@ -2183,21 +2183,21 @@
         <v>2.5935991999999999</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="3">
         <v>50</v>
@@ -2215,21 +2215,21 @@
         <v>3.0595469</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="3">
         <v>107</v>
@@ -2247,21 +2247,21 @@
         <v>3.2323621999999999</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="3">
         <v>109</v>
@@ -2279,21 +2279,21 @@
         <v>2.8712141999999998</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="3">
         <v>19</v>
@@ -2311,21 +2311,21 @@
         <v>2.6410646999999998</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24" s="7">
         <v>63</v>
@@ -2344,7 +2344,7 @@
         <v>3.45</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>